<commit_message>
add board info in openeuler 22.03 LTS
1. SR130 inherits SR130-M board info and SR130-M inherits SR130
   board info;
2. add PMC3152 board info in aarch64 and x86_64 in openeuler 22.03 LTS;
3. add SR450C-M board info in aarch64 and x86_64 in openeuler 22.03 LTS
4. add SR450C-M board info in aarch64 and x86_64 in openeuler 20.03 LTS SP3
5. add RU130 board info in openeuler 22.03 LTS
6. add SmartHBA board info in openeuler 22.03 LTS
7. add six board info in openeuler 22.03 LTS
8. add three board info in openeuler 20.03 LTS SP3
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler20.03-LTS-SP1上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler20.03-LTS-SP1上两类平台板卡兼容清单.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" tabRatio="603"/>
+    <workbookView windowWidth="20925" windowHeight="9750" tabRatio="603"/>
   </bookViews>
   <sheets>
     <sheet name="openEuler20.03-LTS-SP1两类平台板卡兼容性" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'openEuler20.03-LTS-SP1两类平台板卡兼容性'!$A$1:$Q$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'openEuler20.03-LTS-SP1两类平台板卡兼容性'!$A$1:$Q$177</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="646">
   <si>
     <t>vendorID</t>
   </si>
@@ -2345,7 +2345,7 @@
     <t>540KB</t>
   </si>
   <si>
-    <t>SAS9311-8i</t>
+    <t>SR130</t>
   </si>
   <si>
     <t xml:space="preserve">SAS3008 </t>
@@ -3253,9 +3253,6 @@
     <t>PMC8222</t>
   </si>
   <si>
-    <t>SR130</t>
-  </si>
-  <si>
     <t>RU130</t>
   </si>
   <si>
@@ -3263,6 +3260,9 @@
   </si>
   <si>
     <t>SR130-M</t>
+  </si>
+  <si>
+    <t>03023QGH</t>
   </si>
   <si>
     <t>SR430C</t>
@@ -4617,13 +4617,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:R178"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:R177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F181" sqref="F181"/>
+      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4633,17 +4633,17 @@
     <col min="3" max="3" width="8.75" style="15" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.25" style="15" customWidth="1"/>
-    <col min="6" max="6" width="27.5" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="15" customWidth="1"/>
-    <col min="8" max="8" width="24.875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="27.5" style="15" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.25" style="15" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.875" style="15" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="15" customWidth="1"/>
-    <col min="10" max="10" width="13.125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="65" style="15" customWidth="1"/>
-    <col min="12" max="12" width="16.625" style="15" customWidth="1"/>
-    <col min="13" max="13" width="17.375" style="15" customWidth="1"/>
-    <col min="14" max="14" width="32.75" style="15" customWidth="1"/>
-    <col min="15" max="15" width="42" style="15" customWidth="1"/>
-    <col min="16" max="16" width="22.25" style="16" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="15" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="65" style="15" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.8" style="15" customWidth="1"/>
+    <col min="13" max="13" width="7.30833333333333" style="15" customWidth="1"/>
+    <col min="14" max="14" width="11.4416666666667" style="15" customWidth="1"/>
+    <col min="15" max="15" width="12.0166666666667" style="15" customWidth="1"/>
+    <col min="16" max="16" width="10.475" style="16" customWidth="1"/>
     <col min="17" max="17" width="189" style="15" customWidth="1"/>
     <col min="18" max="16384" width="9" style="15"/>
   </cols>
@@ -4704,7 +4704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" spans="1:17">
+    <row r="2" s="5" customFormat="1" hidden="1" spans="1:17">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" hidden="1" spans="1:17">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" hidden="1" spans="1:17">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" hidden="1" spans="1:17">
       <c r="A5" s="15" t="s">
         <v>19</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" hidden="1" spans="1:17">
       <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" s="6" customFormat="1" ht="14.25" customHeight="1" spans="1:17">
+    <row r="7" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" spans="1:17">
       <c r="A7" s="6" t="s">
         <v>43</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" hidden="1" spans="1:17">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" hidden="1" spans="1:17">
       <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" hidden="1" spans="1:17">
       <c r="A10" s="16">
         <v>1077</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" hidden="1" spans="1:17">
       <c r="A11" s="16">
         <v>1077</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" hidden="1" spans="1:17">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" hidden="1" spans="1:17">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" hidden="1" spans="1:17">
       <c r="A14" s="16">
         <v>1002</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" hidden="1" spans="1:17">
       <c r="A15" s="16">
         <v>1002</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" hidden="1" spans="1:17">
       <c r="A16" s="16">
         <v>1002</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" hidden="1" spans="1:17">
       <c r="A17" s="16">
         <v>1002</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" hidden="1" spans="1:17">
       <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" hidden="1" spans="1:17">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" ht="14.1" customHeight="1" spans="1:17">
+    <row r="20" ht="14.1" hidden="1" customHeight="1" spans="1:17">
       <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" hidden="1" spans="1:17">
       <c r="A21" s="15" t="s">
         <v>20</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" hidden="1" spans="1:17">
       <c r="A22" s="15" t="s">
         <v>20</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" hidden="1" spans="1:17">
       <c r="A23" s="15" t="s">
         <v>20</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" hidden="1" spans="1:17">
       <c r="A24" s="15" t="s">
         <v>117</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" hidden="1" spans="1:17">
       <c r="A25" s="16">
         <v>1000</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" hidden="1" spans="1:17">
       <c r="A26" s="16">
         <v>1000</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" hidden="1" spans="1:17">
       <c r="A27" s="15" t="s">
         <v>117</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1" spans="1:17">
+    <row r="28" ht="14.25" hidden="1" customHeight="1" spans="1:17">
       <c r="A28" s="15" t="s">
         <v>117</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" ht="12" customHeight="1" spans="1:17">
+    <row r="29" ht="12" hidden="1" customHeight="1" spans="1:17">
       <c r="A29" s="15" t="s">
         <v>147</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" hidden="1" spans="1:17">
       <c r="A30" s="15" t="s">
         <v>147</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" customHeight="1" spans="1:17">
+    <row r="31" hidden="1" customHeight="1" spans="1:17">
       <c r="A31" s="15" t="s">
         <v>147</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="32" s="6" customFormat="1" spans="1:17">
+    <row r="32" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A32" s="6" t="s">
         <v>20</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" s="6" customFormat="1" spans="1:17">
+    <row r="33" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A33" s="6" t="s">
         <v>20</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" s="7" customFormat="1" spans="1:17">
+    <row r="34" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A34" s="15" t="s">
         <v>20</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" s="6" customFormat="1" spans="1:17">
+    <row r="35" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A35" s="6" t="s">
         <v>20</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" hidden="1" spans="1:17">
       <c r="A36" s="15">
         <v>1000</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" hidden="1" spans="1:17">
       <c r="A37" s="16">
         <v>1000</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" hidden="1" spans="1:17">
       <c r="A38" s="16">
         <v>1000</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" hidden="1" spans="1:17">
       <c r="A39" s="16">
         <v>1000</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" hidden="1" spans="1:17">
       <c r="A40" s="16" t="s">
         <v>19</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" hidden="1" spans="1:17">
       <c r="A41" s="16" t="s">
         <v>19</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" hidden="1" spans="1:17">
       <c r="A42" s="16" t="s">
         <v>19</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" hidden="1" spans="1:17">
       <c r="A43" s="16" t="s">
         <v>19</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" ht="14.25" customHeight="1" spans="1:17">
+    <row r="44" ht="14.25" hidden="1" customHeight="1" spans="1:17">
       <c r="A44" s="16" t="s">
         <v>19</v>
       </c>
@@ -6979,7 +6979,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" hidden="1" spans="1:17">
       <c r="A45" s="16">
         <v>8086</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" hidden="1" spans="1:17">
       <c r="A46" s="16">
         <v>8086</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" hidden="1" spans="1:17">
       <c r="A47" s="16">
         <v>8086</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" s="8" customFormat="1" spans="1:17">
+    <row r="48" s="8" customFormat="1" hidden="1" spans="1:17">
       <c r="A48" s="24" t="s">
         <v>20</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" s="9" customFormat="1" spans="1:17">
+    <row r="49" s="9" customFormat="1" hidden="1" spans="1:17">
       <c r="A49" s="24" t="s">
         <v>20</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="50" s="6" customFormat="1" spans="1:17">
+    <row r="50" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A50" s="6" t="s">
         <v>43</v>
       </c>
@@ -7291,7 +7291,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" s="6" customFormat="1" spans="1:17">
+    <row r="51" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A51" s="6" t="s">
         <v>43</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" hidden="1" spans="1:17">
       <c r="A52" s="16">
         <v>1000</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" hidden="1" spans="1:17">
       <c r="A53" s="16" t="s">
         <v>147</v>
       </c>
@@ -7444,7 +7444,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" hidden="1" spans="1:17">
       <c r="A54" s="16" t="s">
         <v>147</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="55" s="10" customFormat="1" spans="1:17">
+    <row r="55" s="10" customFormat="1" hidden="1" spans="1:17">
       <c r="A55" s="16">
         <v>8086</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" hidden="1" spans="1:17">
       <c r="A56" s="16">
         <v>8086</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" hidden="1" spans="1:17">
       <c r="A57" s="15" t="s">
         <v>19</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" s="9" customFormat="1" spans="1:17">
+    <row r="58" s="9" customFormat="1" hidden="1" spans="1:17">
       <c r="A58" s="8" t="s">
         <v>19</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" hidden="1" spans="1:17">
       <c r="A59" s="15" t="s">
         <v>265</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" hidden="1" spans="1:17">
       <c r="A60" s="15" t="s">
         <v>265</v>
       </c>
@@ -7806,7 +7806,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" hidden="1" spans="1:17">
       <c r="A61" s="16">
         <v>8086</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" hidden="1" spans="1:17">
       <c r="A62" s="16">
         <v>1000</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" hidden="1" spans="1:17">
       <c r="A63" s="15" t="s">
         <v>147</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" s="8" customFormat="1" spans="1:17">
+    <row r="64" s="8" customFormat="1" hidden="1" spans="1:17">
       <c r="A64" s="24" t="s">
         <v>20</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" s="8" customFormat="1" spans="1:17">
+    <row r="65" s="8" customFormat="1" hidden="1" spans="1:17">
       <c r="A65" s="24" t="s">
         <v>20</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" s="7" customFormat="1" spans="1:17">
+    <row r="66" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A66" s="7" t="s">
         <v>19</v>
       </c>
@@ -8118,7 +8118,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" s="7" customFormat="1" spans="1:17">
+    <row r="67" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A67" s="7" t="s">
         <v>19</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" s="7" customFormat="1" spans="1:17">
+    <row r="68" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A68" s="8">
         <v>8086</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="69" s="11" customFormat="1" spans="1:17">
+    <row r="69" s="11" customFormat="1" hidden="1" spans="1:17">
       <c r="A69" s="8" t="s">
         <v>20</v>
       </c>
@@ -8277,7 +8277,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" s="11" customFormat="1" spans="1:17">
+    <row r="70" s="11" customFormat="1" hidden="1" spans="1:17">
       <c r="A70" s="8" t="s">
         <v>117</v>
       </c>
@@ -8330,7 +8330,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="71" s="11" customFormat="1" spans="1:17">
+    <row r="71" s="11" customFormat="1" hidden="1" spans="1:17">
       <c r="A71" s="8">
         <v>8086</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="72" s="11" customFormat="1" spans="1:17">
+    <row r="72" s="11" customFormat="1" hidden="1" spans="1:17">
       <c r="A72" s="8" t="s">
         <v>19</v>
       </c>
@@ -8434,7 +8434,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" hidden="1" spans="1:17">
       <c r="A73" s="8">
         <v>8086</v>
       </c>
@@ -8485,7 +8485,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" hidden="1" spans="1:17">
       <c r="A74" s="8">
         <v>8086</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" hidden="1" spans="1:17">
       <c r="A75" s="8">
         <v>8086</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" hidden="1" spans="1:17">
       <c r="A76" s="8">
         <v>8086</v>
       </c>
@@ -8638,7 +8638,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" hidden="1" spans="1:17">
       <c r="A77" s="8">
         <v>8086</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" hidden="1" spans="1:17">
       <c r="A78" s="8">
         <v>8086</v>
       </c>
@@ -8740,7 +8740,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" hidden="1" spans="1:17">
       <c r="A79" s="8">
         <v>9005</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="80" s="12" customFormat="1" spans="1:17">
+    <row r="80" s="12" customFormat="1" hidden="1" spans="1:17">
       <c r="A80" s="8" t="s">
         <v>147</v>
       </c>
@@ -8842,7 +8842,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" ht="14.1" customHeight="1" spans="1:17">
+    <row r="81" ht="14.1" hidden="1" customHeight="1" spans="1:17">
       <c r="A81" s="8" t="s">
         <v>19</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" hidden="1" spans="1:17">
       <c r="A82" s="8" t="s">
         <v>19</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" hidden="1" spans="1:17">
       <c r="A83" s="8" t="s">
         <v>19</v>
       </c>
@@ -8995,7 +8995,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" hidden="1" spans="1:17">
       <c r="A84" s="8" t="s">
         <v>19</v>
       </c>
@@ -9046,7 +9046,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" hidden="1" spans="1:17">
       <c r="A85" s="15" t="s">
         <v>19</v>
       </c>
@@ -9096,7 +9096,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" hidden="1" spans="1:17">
       <c r="A86" s="15" t="s">
         <v>19</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" hidden="1" spans="1:17">
       <c r="A87" s="15" t="s">
         <v>19</v>
       </c>
@@ -9196,7 +9196,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" hidden="1" spans="1:17">
       <c r="A88" s="15">
         <v>8086</v>
       </c>
@@ -9246,7 +9246,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" hidden="1" spans="1:17">
       <c r="A89" s="15">
         <v>8086</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="90" s="13" customFormat="1" spans="1:17">
+    <row r="90" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A90" s="38">
         <v>8086</v>
       </c>
@@ -9347,7 +9347,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="91" s="13" customFormat="1" spans="1:17">
+    <row r="91" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A91" s="38" t="s">
         <v>117</v>
       </c>
@@ -9398,7 +9398,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="92" s="13" customFormat="1" spans="1:17">
+    <row r="92" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A92" s="13">
         <v>1077</v>
       </c>
@@ -9448,7 +9448,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" s="13" customFormat="1" spans="1:17">
+    <row r="93" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A93" s="13">
         <v>1077</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="94" s="13" customFormat="1" spans="1:17">
+    <row r="94" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A94" s="13">
         <v>1077</v>
       </c>
@@ -9548,7 +9548,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="95" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:17">
+    <row r="95" s="13" customFormat="1" ht="16.5" hidden="1" customHeight="1" spans="1:17">
       <c r="A95" s="40" t="s">
         <v>427</v>
       </c>
@@ -9599,7 +9599,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="96" s="13" customFormat="1" spans="1:17">
+    <row r="96" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A96" s="40" t="s">
         <v>427</v>
       </c>
@@ -9649,7 +9649,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" s="11" customFormat="1" spans="1:17">
+    <row r="97" s="11" customFormat="1" hidden="1" spans="1:17">
       <c r="A97" s="8" t="s">
         <v>117</v>
       </c>
@@ -9700,7 +9700,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="98" s="14" customFormat="1" spans="1:17">
+    <row r="98" s="14" customFormat="1" hidden="1" spans="1:17">
       <c r="A98" s="14" t="s">
         <v>19</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:17">
+    <row r="100" hidden="1" spans="1:17">
       <c r="A100" s="15" t="s">
         <v>147</v>
       </c>
@@ -9853,7 +9853,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="101" s="14" customFormat="1" spans="1:17">
+    <row r="101" s="14" customFormat="1" hidden="1" spans="1:17">
       <c r="A101" s="14" t="s">
         <v>19</v>
       </c>
@@ -9903,7 +9903,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" s="6" customFormat="1" spans="1:18">
+    <row r="102" s="6" customFormat="1" hidden="1" spans="1:18">
       <c r="A102" s="6" t="s">
         <v>43</v>
       </c>
@@ -9956,7 +9956,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" hidden="1" spans="1:18">
       <c r="A103" s="15" t="s">
         <v>265</v>
       </c>
@@ -10012,7 +10012,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="104" spans="1:17">
+    <row r="104" hidden="1" spans="1:17">
       <c r="A104" s="15" t="s">
         <v>265</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="105" s="6" customFormat="1" spans="1:17">
+    <row r="105" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A105" s="6" t="s">
         <v>43</v>
       </c>
@@ -10115,7 +10115,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="106" s="6" customFormat="1" spans="1:17">
+    <row r="106" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A106" s="6" t="s">
         <v>43</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="107" s="13" customFormat="1" spans="1:17">
+    <row r="107" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A107" s="40" t="s">
         <v>20</v>
       </c>
@@ -10218,7 +10218,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="108" s="7" customFormat="1" spans="1:17">
+    <row r="108" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A108" s="36">
         <v>1000</v>
       </c>
@@ -10271,7 +10271,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="109" s="7" customFormat="1" spans="1:17">
+    <row r="109" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A109" s="36">
         <v>1000</v>
       </c>
@@ -10322,7 +10322,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="110" s="6" customFormat="1" spans="1:17">
+    <row r="110" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A110" s="25" t="s">
         <v>43</v>
       </c>
@@ -10372,7 +10372,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="111" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:17">
+    <row r="111" s="13" customFormat="1" ht="16.5" hidden="1" customHeight="1" spans="1:17">
       <c r="A111" s="40" t="s">
         <v>427</v>
       </c>
@@ -10423,7 +10423,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" s="13" customFormat="1" spans="1:17">
+    <row r="112" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A112" s="40" t="s">
         <v>427</v>
       </c>
@@ -10473,7 +10473,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" s="13" customFormat="1" spans="1:17">
+    <row r="113" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A113" s="40" t="s">
         <v>500</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="114" s="13" customFormat="1" spans="1:17">
+    <row r="114" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A114" s="40" t="s">
         <v>500</v>
       </c>
@@ -10579,7 +10579,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" hidden="1" spans="1:17">
       <c r="A115" s="8" t="s">
         <v>117</v>
       </c>
@@ -10632,7 +10632,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" hidden="1" spans="1:17">
       <c r="A116" s="45" t="s">
         <v>513</v>
       </c>
@@ -10677,7 +10677,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" hidden="1" spans="1:17">
       <c r="A117" s="49">
         <v>8088</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" hidden="1" spans="1:17">
       <c r="A118" s="45" t="s">
         <v>513</v>
       </c>
@@ -10772,7 +10772,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" hidden="1" spans="1:17">
       <c r="A119" s="49">
         <v>8088</v>
       </c>
@@ -10822,7 +10822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" s="7" customFormat="1" spans="1:17">
+    <row r="120" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A120" s="27" t="s">
         <v>19</v>
       </c>
@@ -10873,7 +10873,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" s="7" customFormat="1" spans="1:17">
+    <row r="121" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A121" s="7" t="s">
         <v>19</v>
       </c>
@@ -10923,7 +10923,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="122" s="7" customFormat="1" spans="1:17">
+    <row r="122" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A122" s="27" t="s">
         <v>20</v>
       </c>
@@ -10974,7 +10974,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="123" s="7" customFormat="1" spans="1:17">
+    <row r="123" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A123" s="36" t="s">
         <v>19</v>
       </c>
@@ -11024,7 +11024,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="124" s="7" customFormat="1" spans="1:17">
+    <row r="124" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A124" s="27" t="s">
         <v>19</v>
       </c>
@@ -11074,7 +11074,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:17">
+    <row r="125" hidden="1" spans="1:17">
       <c r="A125" s="8" t="s">
         <v>540</v>
       </c>
@@ -11125,7 +11125,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="126" spans="1:17">
+    <row r="126" hidden="1" spans="1:17">
       <c r="A126" s="8">
         <v>1000</v>
       </c>
@@ -11176,7 +11176,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="127" s="7" customFormat="1" spans="1:17">
+    <row r="127" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A127" s="27" t="s">
         <v>19</v>
       </c>
@@ -11227,7 +11227,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:17">
+    <row r="128" hidden="1" spans="1:17">
       <c r="A128" s="8" t="s">
         <v>20</v>
       </c>
@@ -11278,7 +11278,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="129" spans="1:17">
+    <row r="129" hidden="1" spans="1:17">
       <c r="A129" s="8">
         <v>1000</v>
       </c>
@@ -11329,7 +11329,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="130" spans="1:17">
+    <row r="130" hidden="1" spans="1:17">
       <c r="A130" s="8">
         <v>1000</v>
       </c>
@@ -11380,7 +11380,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="131" s="13" customFormat="1" spans="1:17">
+    <row r="131" s="13" customFormat="1" hidden="1" spans="1:17">
       <c r="A131" s="40" t="s">
         <v>20</v>
       </c>
@@ -11433,7 +11433,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="132" s="7" customFormat="1" spans="1:17">
+    <row r="132" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A132" s="7" t="s">
         <v>19</v>
       </c>
@@ -11483,7 +11483,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="133" s="7" customFormat="1" spans="1:17">
+    <row r="133" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A133" s="27" t="s">
         <v>19</v>
       </c>
@@ -11533,7 +11533,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="134" s="7" customFormat="1" spans="1:17">
+    <row r="134" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A134" s="7" t="s">
         <v>19</v>
       </c>
@@ -11583,7 +11583,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="135" s="7" customFormat="1" spans="1:17">
+    <row r="135" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A135" s="27" t="s">
         <v>20</v>
       </c>
@@ -11633,7 +11633,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="136" s="7" customFormat="1" spans="1:17">
+    <row r="136" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A136" s="27" t="s">
         <v>19</v>
       </c>
@@ -11683,7 +11683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="137" s="7" customFormat="1" spans="1:17">
+    <row r="137" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A137" s="27" t="s">
         <v>429</v>
       </c>
@@ -11733,7 +11733,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="138" s="7" customFormat="1" spans="1:17">
+    <row r="138" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A138" s="27" t="s">
         <v>19</v>
       </c>
@@ -11783,7 +11783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="139" s="7" customFormat="1" spans="1:17">
+    <row r="139" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A139" s="36">
         <v>1000</v>
       </c>
@@ -11836,7 +11836,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="140" s="7" customFormat="1" spans="1:17">
+    <row r="140" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A140" s="27">
         <v>1000</v>
       </c>
@@ -11886,7 +11886,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="141" spans="1:17">
+    <row r="141" hidden="1" spans="1:17">
       <c r="A141" s="15" t="s">
         <v>580</v>
       </c>
@@ -11936,7 +11936,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="142" s="7" customFormat="1" spans="1:17">
+    <row r="142" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A142" s="7" t="s">
         <v>359</v>
       </c>
@@ -11984,7 +11984,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="143" s="7" customFormat="1" spans="1:17">
+    <row r="143" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A143" s="7" t="s">
         <v>359</v>
       </c>
@@ -12032,7 +12032,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="144" s="6" customFormat="1" spans="1:17">
+    <row r="144" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A144" s="25" t="s">
         <v>43</v>
       </c>
@@ -12082,7 +12082,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="145" s="6" customFormat="1" spans="1:17">
+    <row r="145" s="6" customFormat="1" hidden="1" spans="1:17">
       <c r="A145" s="25" t="s">
         <v>43</v>
       </c>
@@ -12132,7 +12132,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="146" s="7" customFormat="1" spans="1:17">
+    <row r="146" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A146" s="7" t="s">
         <v>117</v>
       </c>
@@ -12180,7 +12180,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" s="7" customFormat="1" spans="1:17">
+    <row r="147" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A147" s="7" t="s">
         <v>117</v>
       </c>
@@ -12228,7 +12228,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="148" s="7" customFormat="1" spans="1:17">
+    <row r="148" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A148" s="7" t="s">
         <v>540</v>
       </c>
@@ -12281,7 +12281,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="149" spans="1:17">
+    <row r="149" hidden="1" spans="1:17">
       <c r="A149" s="15" t="s">
         <v>580</v>
       </c>
@@ -12328,7 +12328,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="150" spans="1:17">
+    <row r="150" hidden="1" spans="1:17">
       <c r="A150" s="15" t="s">
         <v>60</v>
       </c>
@@ -12378,7 +12378,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="151" spans="1:17">
+    <row r="151" hidden="1" spans="1:17">
       <c r="A151" s="15" t="s">
         <v>60</v>
       </c>
@@ -12428,7 +12428,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="152" spans="1:17">
+    <row r="152" hidden="1" spans="1:17">
       <c r="A152" s="15" t="s">
         <v>60</v>
       </c>
@@ -12478,7 +12478,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="153" spans="1:17">
+    <row r="153" hidden="1" spans="1:17">
       <c r="A153" s="15" t="s">
         <v>60</v>
       </c>
@@ -12528,7 +12528,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="154" s="7" customFormat="1" spans="1:17">
+    <row r="154" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A154" s="7" t="s">
         <v>359</v>
       </c>
@@ -12576,7 +12576,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="155" s="7" customFormat="1" spans="1:17">
+    <row r="155" s="7" customFormat="1" hidden="1" spans="1:17">
       <c r="A155" s="7" t="s">
         <v>359</v>
       </c>
@@ -12624,7 +12624,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="156" s="13" customFormat="1" ht="15" customHeight="1" spans="1:17">
+    <row r="156" s="13" customFormat="1" ht="15" hidden="1" customHeight="1" spans="1:17">
       <c r="A156" s="7">
         <v>1000</v>
       </c>
@@ -12685,8 +12685,8 @@
       <c r="C157" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="D157" s="7">
-        <v>3090</v>
+      <c r="D157" s="7" t="s">
+        <v>630</v>
       </c>
       <c r="E157" s="40" t="s">
         <v>22</v>
@@ -12716,103 +12716,102 @@
         <v>133</v>
       </c>
       <c r="N157" s="40" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="O157" s="40" t="s">
         <v>449</v>
       </c>
-      <c r="P157" s="40"/>
+      <c r="P157" s="40" t="s">
+        <v>632</v>
+      </c>
       <c r="Q157" s="40" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="158" s="13" customFormat="1" ht="15" customHeight="1" spans="1:17">
-      <c r="A158" s="7">
+    <row r="158" hidden="1" spans="1:17">
+      <c r="A158" s="8">
         <v>1000</v>
       </c>
-      <c r="B158" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="C158" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="D158" s="7" t="s">
-        <v>631</v>
-      </c>
-      <c r="E158" s="40" t="s">
+      <c r="B158" s="24" t="s">
+        <v>560</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D158" s="8" t="s">
+        <v>561</v>
+      </c>
+      <c r="E158" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F158" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="G158" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="H158" s="40" t="s">
-        <v>445</v>
-      </c>
-      <c r="I158" s="40" t="s">
+      <c r="F158" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="G158" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H158" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="I158" s="8" t="s">
         <v>131</v>
       </c>
       <c r="J158" s="8" t="s">
-        <v>446</v>
-      </c>
-      <c r="K158" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="L158" s="40" t="s">
-        <v>447</v>
-      </c>
-      <c r="M158" s="40" t="s">
+        <v>563</v>
+      </c>
+      <c r="K158" s="8"/>
+      <c r="L158" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="M158" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="N158" s="40" t="s">
-        <v>632</v>
-      </c>
-      <c r="O158" s="40" t="s">
-        <v>449</v>
-      </c>
-      <c r="P158" s="40"/>
-      <c r="Q158" s="40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="159" spans="1:17">
-      <c r="A159" s="8">
+      <c r="N158" s="8" t="s">
+        <v>633</v>
+      </c>
+      <c r="O158" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="P158" s="8"/>
+      <c r="Q158" s="32" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="159" s="7" customFormat="1" hidden="1" spans="1:17">
+      <c r="A159" s="27">
         <v>1000</v>
       </c>
-      <c r="B159" s="24" t="s">
+      <c r="B159" s="37" t="s">
         <v>560</v>
       </c>
-      <c r="C159" s="8" t="s">
+      <c r="C159" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D159" s="8" t="s">
+      <c r="D159" s="27" t="s">
         <v>561</v>
       </c>
-      <c r="E159" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F159" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="G159" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H159" s="8" t="s">
+      <c r="E159" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F159" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G159" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="H159" s="27" t="s">
         <v>542</v>
       </c>
-      <c r="I159" s="8" t="s">
+      <c r="I159" s="27" t="s">
         <v>131</v>
       </c>
       <c r="J159" s="8" t="s">
-        <v>563</v>
-      </c>
-      <c r="K159" s="8"/>
-      <c r="L159" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="L159" s="27" t="s">
         <v>549</v>
       </c>
-      <c r="M159" s="8" t="s">
+      <c r="M159" s="27" t="s">
         <v>133</v>
       </c>
       <c r="N159" s="8" t="s">
@@ -12822,94 +12821,94 @@
         <v>565</v>
       </c>
       <c r="P159" s="8"/>
-      <c r="Q159" s="32" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="160" s="7" customFormat="1" spans="1:17">
-      <c r="A160" s="27">
+      <c r="Q159" s="27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="160" hidden="1" spans="1:17">
+      <c r="A160" s="8">
         <v>1000</v>
       </c>
-      <c r="B160" s="37" t="s">
+      <c r="B160" s="24" t="s">
         <v>560</v>
       </c>
-      <c r="C160" s="27" t="s">
+      <c r="C160" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D160" s="27" t="s">
+      <c r="D160" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="E160" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F160" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G160" s="27" t="s">
-        <v>577</v>
-      </c>
-      <c r="H160" s="27" t="s">
+      <c r="E160" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F160" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="G160" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H160" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="I160" s="27" t="s">
+      <c r="I160" s="8" t="s">
         <v>131</v>
       </c>
       <c r="J160" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="L160" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="K160" s="8"/>
+      <c r="L160" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="M160" s="27" t="s">
+      <c r="M160" s="8" t="s">
         <v>133</v>
       </c>
       <c r="N160" s="8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="O160" s="8" t="s">
         <v>565</v>
       </c>
       <c r="P160" s="8"/>
-      <c r="Q160" s="27" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="161" spans="1:17">
-      <c r="A161" s="8">
+      <c r="Q160" s="32" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="161" s="7" customFormat="1" hidden="1" spans="1:17">
+      <c r="A161" s="27">
         <v>1000</v>
       </c>
-      <c r="B161" s="24" t="s">
+      <c r="B161" s="37" t="s">
         <v>560</v>
       </c>
-      <c r="C161" s="8" t="s">
+      <c r="C161" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D161" s="8" t="s">
+      <c r="D161" s="27" t="s">
         <v>561</v>
       </c>
-      <c r="E161" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F161" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="G161" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H161" s="8" t="s">
+      <c r="E161" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F161" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G161" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="H161" s="27" t="s">
         <v>542</v>
       </c>
-      <c r="I161" s="8" t="s">
+      <c r="I161" s="27" t="s">
         <v>131</v>
       </c>
       <c r="J161" s="8" t="s">
-        <v>563</v>
-      </c>
-      <c r="K161" s="8"/>
-      <c r="L161" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="L161" s="27" t="s">
         <v>549</v>
       </c>
-      <c r="M161" s="8" t="s">
+      <c r="M161" s="27" t="s">
         <v>133</v>
       </c>
       <c r="N161" s="8" t="s">
@@ -12919,94 +12918,94 @@
         <v>565</v>
       </c>
       <c r="P161" s="8"/>
-      <c r="Q161" s="32" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="162" s="7" customFormat="1" spans="1:17">
-      <c r="A162" s="27">
+      <c r="Q161" s="27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="162" hidden="1" spans="1:17">
+      <c r="A162" s="8">
         <v>1000</v>
       </c>
-      <c r="B162" s="37" t="s">
+      <c r="B162" s="24" t="s">
         <v>560</v>
       </c>
-      <c r="C162" s="27" t="s">
+      <c r="C162" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D162" s="27" t="s">
+      <c r="D162" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="E162" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F162" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G162" s="27" t="s">
-        <v>577</v>
-      </c>
-      <c r="H162" s="27" t="s">
+      <c r="E162" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F162" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="G162" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H162" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="I162" s="27" t="s">
+      <c r="I162" s="8" t="s">
         <v>131</v>
       </c>
       <c r="J162" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="L162" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="K162" s="8"/>
+      <c r="L162" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="M162" s="27" t="s">
+      <c r="M162" s="8" t="s">
         <v>133</v>
       </c>
       <c r="N162" s="8" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="O162" s="8" t="s">
         <v>565</v>
       </c>
       <c r="P162" s="8"/>
-      <c r="Q162" s="27" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="163" spans="1:17">
-      <c r="A163" s="8">
+      <c r="Q162" s="32" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="163" s="7" customFormat="1" hidden="1" spans="1:17">
+      <c r="A163" s="27">
         <v>1000</v>
       </c>
-      <c r="B163" s="24" t="s">
+      <c r="B163" s="37" t="s">
         <v>560</v>
       </c>
-      <c r="C163" s="8" t="s">
+      <c r="C163" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D163" s="8" t="s">
+      <c r="D163" s="27" t="s">
         <v>561</v>
       </c>
-      <c r="E163" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F163" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="G163" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H163" s="8" t="s">
+      <c r="E163" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F163" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G163" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="H163" s="27" t="s">
         <v>542</v>
       </c>
-      <c r="I163" s="8" t="s">
+      <c r="I163" s="27" t="s">
         <v>131</v>
       </c>
       <c r="J163" s="8" t="s">
-        <v>563</v>
-      </c>
-      <c r="K163" s="8"/>
-      <c r="L163" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="L163" s="27" t="s">
         <v>549</v>
       </c>
-      <c r="M163" s="8" t="s">
+      <c r="M163" s="27" t="s">
         <v>133</v>
       </c>
       <c r="N163" s="8" t="s">
@@ -13016,94 +13015,94 @@
         <v>565</v>
       </c>
       <c r="P163" s="8"/>
-      <c r="Q163" s="32" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="164" s="7" customFormat="1" spans="1:17">
-      <c r="A164" s="27">
+      <c r="Q163" s="27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="164" hidden="1" spans="1:17">
+      <c r="A164" s="8">
         <v>1000</v>
       </c>
-      <c r="B164" s="37" t="s">
+      <c r="B164" s="24" t="s">
         <v>560</v>
       </c>
-      <c r="C164" s="27" t="s">
+      <c r="C164" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D164" s="27" t="s">
-        <v>561</v>
-      </c>
-      <c r="E164" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F164" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G164" s="27" t="s">
-        <v>577</v>
-      </c>
-      <c r="H164" s="27" t="s">
+      <c r="D164" s="8" t="s">
+        <v>636</v>
+      </c>
+      <c r="E164" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F164" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="G164" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H164" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="I164" s="27" t="s">
+      <c r="I164" s="8" t="s">
         <v>131</v>
       </c>
       <c r="J164" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="L164" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="K164" s="8"/>
+      <c r="L164" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="M164" s="27" t="s">
+      <c r="M164" s="8" t="s">
         <v>133</v>
       </c>
       <c r="N164" s="8" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="O164" s="8" t="s">
         <v>565</v>
       </c>
       <c r="P164" s="8"/>
-      <c r="Q164" s="27" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="165" spans="1:17">
-      <c r="A165" s="8">
+      <c r="Q164" s="32" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="165" s="7" customFormat="1" hidden="1" spans="1:17">
+      <c r="A165" s="27">
         <v>1000</v>
       </c>
-      <c r="B165" s="24" t="s">
+      <c r="B165" s="37" t="s">
         <v>560</v>
       </c>
-      <c r="C165" s="8" t="s">
+      <c r="C165" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D165" s="8" t="s">
-        <v>636</v>
-      </c>
-      <c r="E165" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F165" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="G165" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H165" s="8" t="s">
+      <c r="D165" s="27" t="s">
+        <v>638</v>
+      </c>
+      <c r="E165" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F165" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G165" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="H165" s="27" t="s">
         <v>542</v>
       </c>
-      <c r="I165" s="8" t="s">
+      <c r="I165" s="27" t="s">
         <v>131</v>
       </c>
       <c r="J165" s="8" t="s">
-        <v>563</v>
-      </c>
-      <c r="K165" s="8"/>
-      <c r="L165" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="L165" s="27" t="s">
         <v>549</v>
       </c>
-      <c r="M165" s="8" t="s">
+      <c r="M165" s="27" t="s">
         <v>133</v>
       </c>
       <c r="N165" s="8" t="s">
@@ -13113,94 +13112,94 @@
         <v>565</v>
       </c>
       <c r="P165" s="8"/>
-      <c r="Q165" s="32" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="166" s="7" customFormat="1" spans="1:17">
-      <c r="A166" s="27">
+      <c r="Q165" s="27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="166" hidden="1" spans="1:17">
+      <c r="A166" s="8">
         <v>1000</v>
       </c>
-      <c r="B166" s="37" t="s">
+      <c r="B166" s="24" t="s">
         <v>560</v>
       </c>
-      <c r="C166" s="27" t="s">
+      <c r="C166" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D166" s="27" t="s">
-        <v>638</v>
-      </c>
-      <c r="E166" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F166" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G166" s="27" t="s">
-        <v>577</v>
-      </c>
-      <c r="H166" s="27" t="s">
+      <c r="D166" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="E166" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F166" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="G166" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H166" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="I166" s="27" t="s">
+      <c r="I166" s="8" t="s">
         <v>131</v>
       </c>
       <c r="J166" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="L166" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="K166" s="8"/>
+      <c r="L166" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="M166" s="27" t="s">
+      <c r="M166" s="8" t="s">
         <v>133</v>
       </c>
       <c r="N166" s="8" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="O166" s="8" t="s">
         <v>565</v>
       </c>
       <c r="P166" s="8"/>
-      <c r="Q166" s="27" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="167" spans="1:17">
-      <c r="A167" s="8">
+      <c r="Q166" s="32" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="167" s="7" customFormat="1" hidden="1" spans="1:17">
+      <c r="A167" s="27">
         <v>1000</v>
       </c>
-      <c r="B167" s="24" t="s">
+      <c r="B167" s="37" t="s">
         <v>560</v>
       </c>
-      <c r="C167" s="8" t="s">
+      <c r="C167" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D167" s="8" t="s">
+      <c r="D167" s="27" t="s">
         <v>639</v>
       </c>
-      <c r="E167" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F167" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="G167" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H167" s="8" t="s">
+      <c r="E167" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F167" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G167" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="H167" s="27" t="s">
         <v>542</v>
       </c>
-      <c r="I167" s="8" t="s">
+      <c r="I167" s="27" t="s">
         <v>131</v>
       </c>
       <c r="J167" s="8" t="s">
-        <v>563</v>
-      </c>
-      <c r="K167" s="8"/>
-      <c r="L167" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="L167" s="27" t="s">
         <v>549</v>
       </c>
-      <c r="M167" s="8" t="s">
+      <c r="M167" s="27" t="s">
         <v>133</v>
       </c>
       <c r="N167" s="8" t="s">
@@ -13210,59 +13209,62 @@
         <v>565</v>
       </c>
       <c r="P167" s="8"/>
-      <c r="Q167" s="32" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="168" s="7" customFormat="1" spans="1:17">
-      <c r="A168" s="27">
+      <c r="Q167" s="27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="168" hidden="1" spans="1:17">
+      <c r="A168" s="16">
         <v>1000</v>
       </c>
-      <c r="B168" s="37" t="s">
-        <v>560</v>
-      </c>
-      <c r="C168" s="27" t="s">
+      <c r="B168" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C168" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D168" s="27" t="s">
-        <v>639</v>
-      </c>
-      <c r="E168" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F168" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G168" s="27" t="s">
-        <v>577</v>
-      </c>
-      <c r="H168" s="27" t="s">
-        <v>542</v>
-      </c>
-      <c r="I168" s="27" t="s">
+      <c r="D168" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E168" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F168" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G168" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H168" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="I168" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J168" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="L168" s="27" t="s">
-        <v>549</v>
-      </c>
-      <c r="M168" s="27" t="s">
+      <c r="J168" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="K168" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L168" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="M168" s="8" t="s">
         <v>133</v>
       </c>
       <c r="N168" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="O168" s="8" t="s">
-        <v>565</v>
+        <v>135</v>
       </c>
       <c r="P168" s="8"/>
-      <c r="Q168" s="27" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="169" spans="1:17">
+      <c r="Q168" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="169" hidden="1" spans="1:17">
       <c r="A169" s="16">
         <v>1000</v>
       </c>
@@ -13276,7 +13278,7 @@
         <v>128</v>
       </c>
       <c r="E169" s="15" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F169" s="15" t="s">
         <v>23</v>
@@ -13290,16 +13292,16 @@
       <c r="I169" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J169" s="27" t="s">
-        <v>122</v>
+      <c r="J169" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="K169" s="15" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="L169" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="M169" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="M169" s="15" t="s">
         <v>133</v>
       </c>
       <c r="N169" s="8" t="s">
@@ -13313,7 +13315,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="170" spans="1:17">
+    <row r="170" hidden="1" spans="1:17">
       <c r="A170" s="16">
         <v>1000</v>
       </c>
@@ -13327,7 +13329,7 @@
         <v>128</v>
       </c>
       <c r="E170" s="15" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F170" s="15" t="s">
         <v>23</v>
@@ -13341,20 +13343,20 @@
       <c r="I170" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J170" s="8" t="s">
-        <v>137</v>
+      <c r="J170" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="K170" s="15" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="L170" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="M170" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="M170" s="8" t="s">
         <v>133</v>
       </c>
       <c r="N170" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="O170" s="8" t="s">
         <v>135</v>
@@ -13364,7 +13366,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="171" spans="1:17">
+    <row r="171" hidden="1" spans="1:17">
       <c r="A171" s="16">
         <v>1000</v>
       </c>
@@ -13378,7 +13380,7 @@
         <v>128</v>
       </c>
       <c r="E171" s="15" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F171" s="15" t="s">
         <v>23</v>
@@ -13392,16 +13394,16 @@
       <c r="I171" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J171" s="27" t="s">
-        <v>122</v>
+      <c r="J171" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="K171" s="15" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="L171" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="M171" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="M171" s="15" t="s">
         <v>133</v>
       </c>
       <c r="N171" s="8" t="s">
@@ -13415,18 +13417,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="172" spans="1:17">
+    <row r="172" hidden="1" spans="1:17">
       <c r="A172" s="16">
         <v>1000</v>
       </c>
       <c r="B172" s="16" t="s">
-        <v>127</v>
+        <v>181</v>
       </c>
       <c r="C172" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D172" s="15" t="s">
-        <v>128</v>
+        <v>182</v>
       </c>
       <c r="E172" s="15" t="s">
         <v>35</v>
@@ -13438,72 +13440,72 @@
         <v>129</v>
       </c>
       <c r="H172" s="15" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="I172" s="8" t="s">
         <v>131</v>
       </c>
       <c r="J172" s="8" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="K172" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="L172" s="8" t="s">
-        <v>138</v>
+      <c r="L172" s="30" t="s">
+        <v>179</v>
       </c>
       <c r="M172" s="15" t="s">
         <v>133</v>
       </c>
       <c r="N172" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="O172" s="8" t="s">
-        <v>135</v>
+        <v>643</v>
+      </c>
+      <c r="O172" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="P172" s="8"/>
       <c r="Q172" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="173" spans="1:17">
-      <c r="A173" s="16">
-        <v>1000</v>
-      </c>
-      <c r="B173" s="16" t="s">
+    <row r="173" s="7" customFormat="1" hidden="1" spans="1:17">
+      <c r="A173" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="B173" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C173" s="15" t="s">
+      <c r="C173" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D173" s="15" t="s">
+      <c r="D173" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E173" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F173" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G173" s="15" t="s">
+      <c r="E173" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F173" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G173" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H173" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="I173" s="8" t="s">
+      <c r="H173" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="I173" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="J173" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="K173" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="L173" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="M173" s="15" t="s">
+      <c r="J173" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K173" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="L173" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="M173" s="7" t="s">
         <v>133</v>
       </c>
       <c r="N173" s="8" t="s">
@@ -13513,99 +13515,99 @@
         <v>185</v>
       </c>
       <c r="P173" s="8"/>
-      <c r="Q173" s="15" t="s">
+      <c r="Q173" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="174" s="7" customFormat="1" spans="1:17">
-      <c r="A174" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="B174" s="36" t="s">
+    <row r="174" hidden="1" spans="1:17">
+      <c r="A174" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B174" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="C174" s="7" t="s">
+      <c r="C174" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D174" s="7" t="s">
+      <c r="D174" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="E174" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F174" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G174" s="7" t="s">
+      <c r="E174" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F174" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G174" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="H174" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="I174" s="7" t="s">
+      <c r="H174" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="I174" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J174" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="K174" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="L174" s="7" t="s">
-        <v>606</v>
-      </c>
-      <c r="M174" s="7" t="s">
+      <c r="J174" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="K174" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="L174" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="M174" s="15" t="s">
         <v>133</v>
       </c>
       <c r="N174" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="O174" s="16" t="s">
         <v>185</v>
       </c>
       <c r="P174" s="8"/>
-      <c r="Q174" s="7" t="s">
+      <c r="Q174" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="175" spans="1:17">
-      <c r="A175" s="16">
-        <v>1000</v>
-      </c>
-      <c r="B175" s="16" t="s">
+    <row r="175" s="7" customFormat="1" hidden="1" spans="1:17">
+      <c r="A175" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="B175" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C175" s="15" t="s">
+      <c r="C175" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D175" s="15" t="s">
+      <c r="D175" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E175" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F175" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G175" s="15" t="s">
+      <c r="E175" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F175" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G175" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H175" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="I175" s="8" t="s">
+      <c r="H175" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="I175" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="J175" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="K175" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="L175" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="M175" s="15" t="s">
+      <c r="J175" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K175" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="L175" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="M175" s="7" t="s">
         <v>133</v>
       </c>
       <c r="N175" s="8" t="s">
@@ -13615,165 +13617,121 @@
         <v>185</v>
       </c>
       <c r="P175" s="8"/>
-      <c r="Q175" s="15" t="s">
+      <c r="Q175" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="176" s="7" customFormat="1" spans="1:17">
-      <c r="A176" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="B176" s="36" t="s">
+    <row r="176" hidden="1" spans="1:17">
+      <c r="A176" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B176" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="C176" s="7" t="s">
+      <c r="C176" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D176" s="7" t="s">
+      <c r="D176" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="E176" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F176" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G176" s="7" t="s">
+      <c r="E176" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F176" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G176" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="H176" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="I176" s="7" t="s">
+      <c r="H176" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="I176" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="J176" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="K176" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="L176" s="7" t="s">
-        <v>606</v>
-      </c>
-      <c r="M176" s="7" t="s">
+      <c r="J176" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="K176" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="L176" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="M176" s="15" t="s">
         <v>133</v>
       </c>
       <c r="N176" s="8" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="O176" s="16" t="s">
         <v>185</v>
       </c>
       <c r="P176" s="8"/>
-      <c r="Q176" s="7" t="s">
+      <c r="Q176" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="177" spans="1:17">
-      <c r="A177" s="16">
-        <v>1000</v>
-      </c>
-      <c r="B177" s="16" t="s">
+    <row r="177" s="7" customFormat="1" hidden="1" spans="1:17">
+      <c r="A177" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="B177" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C177" s="15" t="s">
+      <c r="C177" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D177" s="15" t="s">
+      <c r="D177" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E177" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F177" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G177" s="15" t="s">
+      <c r="E177" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F177" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G177" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H177" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="I177" s="8" t="s">
+      <c r="H177" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="I177" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="J177" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="K177" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="L177" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="M177" s="15" t="s">
+      <c r="J177" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K177" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="L177" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="M177" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="N177" s="8" t="s">
+      <c r="N177" s="27" t="s">
         <v>645</v>
       </c>
       <c r="O177" s="16" t="s">
         <v>185</v>
       </c>
       <c r="P177" s="8"/>
-      <c r="Q177" s="15" t="s">
+      <c r="Q177" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="178" s="7" customFormat="1" spans="1:17">
-      <c r="A178" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="B178" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="C178" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D178" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="E178" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F178" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G178" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="H178" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="I178" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="J178" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="K178" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="L178" s="7" t="s">
-        <v>606</v>
-      </c>
-      <c r="M178" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="N178" s="27" t="s">
-        <v>645</v>
-      </c>
-      <c r="O178" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="P178" s="8"/>
-      <c r="Q178" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:Q178">
+  <autoFilter ref="A1:Q177">
+    <filterColumn colId="13">
+      <filters>
+        <filter val="SR130"/>
+        <filter val="SAS9311-8i"/>
+        <filter val="SR130-M"/>
+      </filters>
+    </filterColumn>
     <extLst/>
   </autoFilter>
   <hyperlinks>
@@ -13834,11 +13792,11 @@
     <hyperlink ref="Q121" r:id="rId23" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/source/Packages/MLNX_OFED_LINUX-5.1-2.5.2.0-openeuler20.03-aarch64-ext.tgz"/>
     <hyperlink ref="Q150" r:id="rId28" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/source/Packages/qla2xxx-10.02.06.04_k-1_OpenEuler.zip"/>
     <hyperlink ref="Q151:Q153" r:id="rId28" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/source/Packages/qla2xxx-10.02.06.04_k-1_OpenEuler.zip"/>
-    <hyperlink ref="Q159" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q161" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q163" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q165" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
-    <hyperlink ref="Q167" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
+    <hyperlink ref="Q158" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
+    <hyperlink ref="Q160" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
+    <hyperlink ref="Q162" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
+    <hyperlink ref="Q164" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
+    <hyperlink ref="Q166" r:id="rId21" display="https://repo.oepkgs.net/openEuler/rpm/openEuler-20.03-LTS-SP1/contrib/drivers/x86_64/Packages/RAID-3004iMR_3108_3408iMR_3416iMR_3508_3516-openEuler20.03-megaraid_sas-07.714.04.00-1-x86_64.rpm"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180"/>

</xml_diff>